<commit_message>
update code for update data, export data
</commit_message>
<xml_diff>
--- a/TanoApp/TanoApp/wwwroot/templates/BillTemplate.xlsx
+++ b/TanoApp/TanoApp/wwwroot/templates/BillTemplate.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoct\Documents\Visual Studio 2017\Projects\TeduCore\TeduCore.WebApp\wwwroot\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectHocTap\Net Core\NetCore3_TanoApp\TanoApp\TanoApp\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179588B9-334E-488E-B868-4503BFEB51CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TEDUOrder" sheetId="1" r:id="rId1"/>
+    <sheet name="TanoOrder" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="0"/>
+  <calcPr calcId="191029" iterateDelta="0"/>
 </workbook>
 </file>
 
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -250,44 +251,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -324,7 +325,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -618,7 +625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -635,46 +642,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -883,10 +890,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="3">
         <f>SUM(C9:C23)</f>
         <v>0</v>
@@ -898,32 +905,37 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
@@ -931,11 +943,6 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.55069444444444449" right="0.2361111111111111" top="0.47222222222222221" bottom="0.35416666666666669" header="0.31458333333333333" footer="0.27500000000000002"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" r:id="rId1"/>
@@ -945,7 +952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
@@ -959,7 +966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>

</xml_diff>